<commit_message>
47 pref. list add
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="49">
   <si>
     <t>全国</t>
   </si>
@@ -147,13 +147,55 @@
   </si>
   <si>
     <t>沖縄県</t>
+  </si>
+  <si>
+    <t>青森県</t>
+  </si>
+  <si>
+    <t>岩手県</t>
+  </si>
+  <si>
+    <t>山形県</t>
+  </si>
+  <si>
+    <t>茨城県</t>
+  </si>
+  <si>
+    <t>富山県</t>
+  </si>
+  <si>
+    <t>福井県</t>
+  </si>
+  <si>
+    <t>鳥取県</t>
+  </si>
+  <si>
+    <t>島根県</t>
+  </si>
+  <si>
+    <t>岡山県</t>
+  </si>
+  <si>
+    <t>徳島県</t>
+  </si>
+  <si>
+    <t>香川県</t>
+  </si>
+  <si>
+    <t>佐賀県</t>
+  </si>
+  <si>
+    <t>長崎県</t>
+  </si>
+  <si>
+    <t>鹿児島県</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +210,12 @@
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -207,7 +255,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -219,6 +267,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="P47" sqref="P1:P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -516,7 +567,7 @@
     <col min="6" max="6" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1">
         <v>43898</v>
       </c>
@@ -538,8 +589,27 @@
         <f>C1</f>
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I1" t="str">
+        <f>"      "&amp;"["""&amp;F1&amp;""","&amp;G1&amp;"],"</f>
+        <v xml:space="preserve">      ["北海道",97],</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1">
+        <f>VLOOKUP(L1,B:C,2,FALSE)</f>
+        <v>97</v>
+      </c>
+      <c r="N1">
+        <f>IF(ISNA(M1),0,M1)</f>
+        <v>97</v>
+      </c>
+      <c r="P1" t="str">
+        <f>"      "&amp;"["""&amp;L1&amp;""","&amp;N1&amp;"],"</f>
+        <v xml:space="preserve">      ["北海道",97],</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>43898</v>
       </c>
@@ -561,8 +631,27 @@
         <f t="shared" ref="G2:G33" si="2">C2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I33" si="3">"      "&amp;"["""&amp;F2&amp;""","&amp;G2&amp;"],"</f>
+        <v xml:space="preserve">      ["宮城",1],</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="e">
+        <f t="shared" ref="M2:M47" si="4">VLOOKUP(L2,B:C,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2:N47" si="5">IF(ISNA(M2),0,M2)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" ref="P2:P47" si="6">"      "&amp;"["""&amp;L2&amp;""","&amp;N2&amp;"],"</f>
+        <v xml:space="preserve">      ["青森県",0],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>43898</v>
       </c>
@@ -584,8 +673,27 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I3" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["秋田",1],</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["岩手県",0],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>43898</v>
       </c>
@@ -607,8 +715,27 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["福島",1],</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["宮城県",1],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>43898</v>
       </c>
@@ -630,8 +757,27 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["栃木",2],</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["秋田県",1],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>43898</v>
       </c>
@@ -653,8 +799,27 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I6" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["埼玉",4],</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["山形県",0],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>43898</v>
       </c>
@@ -676,8 +841,27 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["群馬",1],</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["福島県",1],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>43898</v>
       </c>
@@ -699,8 +883,27 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I8" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["千葉",20],</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["茨城県",0],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>43898</v>
       </c>
@@ -722,8 +925,27 @@
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I9" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["東京",60],</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["栃木県",2],</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>43898</v>
       </c>
@@ -745,8 +967,27 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I10" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["神奈川",34],</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["群馬県",1],</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>43898</v>
       </c>
@@ -768,8 +1009,27 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["新潟",6],</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["埼玉県",4],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>43898</v>
       </c>
@@ -791,8 +1051,27 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I12" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["石川",4],</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["千葉県",20],</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>43898</v>
       </c>
@@ -814,8 +1093,27 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I13" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["山梨",2],</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["東京都",60],</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>43898</v>
       </c>
@@ -837,8 +1135,27 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I14" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["長野",2],</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="5"/>
+        <v>34</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["神奈川県",34],</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>43898</v>
       </c>
@@ -860,8 +1177,27 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I15" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["岐阜",2],</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["新潟県",6],</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>43898</v>
       </c>
@@ -883,8 +1219,27 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I16" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["静岡",1],</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["富山県",0],</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>43898</v>
       </c>
@@ -906,8 +1261,27 @@
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I17" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["愛知",68],</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["石川県",4],</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>43898</v>
       </c>
@@ -929,8 +1303,27 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I18" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["三重",1],</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M18" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["福井県",0],</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>43898</v>
       </c>
@@ -952,8 +1345,27 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I19" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["滋賀",1],</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["山梨県",2],</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>43898</v>
       </c>
@@ -975,8 +1387,27 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I20" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["京都",8],</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["長野県",2],</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>43898</v>
       </c>
@@ -998,8 +1429,27 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I21" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["大阪",33],</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["岐阜県",2],</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>43898</v>
       </c>
@@ -1021,8 +1471,27 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I22" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["兵庫",9],</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["静岡県",1],</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>43898</v>
       </c>
@@ -1044,8 +1513,27 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I23" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["奈良",2],</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="4"/>
+        <v>68</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="5"/>
+        <v>68</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["愛知県",68],</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>43898</v>
       </c>
@@ -1067,8 +1555,27 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I24" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["和歌山",12],</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["三重県",1],</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>43898</v>
       </c>
@@ -1090,8 +1597,27 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I25" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["広島",1],</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["滋賀県",1],</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" s="1">
         <v>43898</v>
       </c>
@@ -1113,8 +1639,27 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I26" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["山口",1],</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["京都府",8],</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <v>43898</v>
       </c>
@@ -1136,8 +1681,27 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I27" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["愛媛",1],</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["大阪府",33],</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <v>43898</v>
       </c>
@@ -1159,8 +1723,27 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I28" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["高知",9],</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["兵庫県",9],</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <v>43898</v>
       </c>
@@ -1182,8 +1765,27 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I29" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["福岡",3],</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["奈良県",2],</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.4">
       <c r="A30" s="1">
         <v>43898</v>
       </c>
@@ -1205,8 +1807,27 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I30" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["熊本",5],</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["和歌山県",12],</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <v>43898</v>
       </c>
@@ -1228,8 +1849,27 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I31" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["大分",1],</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M31" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P31" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["鳥取県",0],</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
         <v>43898</v>
       </c>
@@ -1251,8 +1891,27 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="I32" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["宮崎",1],</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M32" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["島根県",0],</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <v>43898</v>
       </c>
@@ -1273,6 +1932,263 @@
       <c r="G33">
         <f t="shared" si="2"/>
         <v>3</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      ["沖縄",3],</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M33" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["岡山県",0],</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="L34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P34" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["広島県",1],</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="L35" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P35" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["山口県",1],</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="L36" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M36" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P36" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["徳島県",0],</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="L37" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M37" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P37" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["香川県",0],</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="L38" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P38" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["愛媛県",1],</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="L39" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="P39" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["高知県",9],</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="L40" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="P40" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["福岡県",3],</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="L41" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M41" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P41" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["佐賀県",0],</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="L42" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M42" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P42" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["長崎県",0],</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="L43" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="P43" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["熊本県",5],</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="L44" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P44" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["大分県",1],</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="L45" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P45" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["宮崎県",1],</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="30" x14ac:dyDescent="0.4">
+      <c r="L46" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M46" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P46" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["鹿児島県",0],</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="L47" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="P47" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">      ["沖縄県",3],</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
47 pref. list edit
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://storyseller1980-my.sharepoint.com/personal/storyseller1980_storyseller1980_onmicrosoft_com/Documents/仕事，勉強/コロナマップ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yikunaga\OneDrive - 個人事業主\仕事，勉強\コロナマップ\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -218,12 +218,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -268,7 +274,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -555,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P47" sqref="P1:P47"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -567,7 +573,7 @@
     <col min="6" max="6" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" s="1">
         <v>43898</v>
       </c>
@@ -596,20 +602,24 @@
       <c r="L1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M1">
+      <c r="M1" t="str">
+        <f>IF(OR(MID(L1,3,1)="県",MID(L1,3,1)="府",MID(L1,3,1)="都"),MID(L1,1,2),MID(L1,1,3))</f>
+        <v>北海道</v>
+      </c>
+      <c r="N1">
         <f>VLOOKUP(L1,B:C,2,FALSE)</f>
         <v>97</v>
       </c>
-      <c r="N1">
-        <f>IF(ISNA(M1),0,M1)</f>
+      <c r="O1">
+        <f>IF(ISNA(N1),0,N1)</f>
         <v>97</v>
       </c>
-      <c r="P1" t="str">
-        <f>"      "&amp;"["""&amp;L1&amp;""","&amp;N1&amp;"],"</f>
+      <c r="Q1" t="str">
+        <f>"      "&amp;"["""&amp;M1&amp;""","&amp;O1&amp;"],"</f>
         <v xml:space="preserve">      ["北海道",97],</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>43898</v>
       </c>
@@ -638,20 +648,24 @@
       <c r="L2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="M2" t="e">
-        <f t="shared" ref="M2:M47" si="4">VLOOKUP(L2,B:C,2,FALSE)</f>
+      <c r="M2" t="str">
+        <f t="shared" ref="M2:M47" si="4">IF(OR(MID(L2,3,1)="県",MID(L2,3,1)="府",MID(L2,3,1)="都"),MID(L2,1,2),MID(L2,1,3))</f>
+        <v>青森</v>
+      </c>
+      <c r="N2" t="e">
+        <f t="shared" ref="N2:N47" si="5">VLOOKUP(L2,B:C,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="N2">
-        <f t="shared" ref="N2:N47" si="5">IF(ISNA(M2),0,M2)</f>
+      <c r="O2">
+        <f t="shared" ref="O2:O47" si="6">IF(ISNA(N2),0,N2)</f>
         <v>0</v>
       </c>
-      <c r="P2" t="str">
-        <f t="shared" ref="P2:P47" si="6">"      "&amp;"["""&amp;L2&amp;""","&amp;N2&amp;"],"</f>
-        <v xml:space="preserve">      ["青森県",0],</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q2" t="str">
+        <f t="shared" ref="Q2:Q47" si="7">"      "&amp;"["""&amp;M2&amp;""","&amp;O2&amp;"],"</f>
+        <v xml:space="preserve">      ["青森",0],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>43898</v>
       </c>
@@ -680,20 +694,24 @@
       <c r="L3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M3" t="e">
-        <f t="shared" si="4"/>
+      <c r="M3" t="str">
+        <f t="shared" si="4"/>
+        <v>岩手</v>
+      </c>
+      <c r="N3" t="e">
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="N3">
-        <f t="shared" si="5"/>
+      <c r="O3">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["岩手県",0],</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q3" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["岩手",0],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>43898</v>
       </c>
@@ -722,20 +740,24 @@
       <c r="L4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M4">
-        <f t="shared" si="4"/>
-        <v>1</v>
+      <c r="M4" t="str">
+        <f t="shared" si="4"/>
+        <v>宮城</v>
       </c>
       <c r="N4">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P4" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["宮城県",1],</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="O4">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["宮城",1],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>43898</v>
       </c>
@@ -764,20 +786,24 @@
       <c r="L5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M5">
-        <f t="shared" si="4"/>
-        <v>1</v>
+      <c r="M5" t="str">
+        <f t="shared" si="4"/>
+        <v>秋田</v>
       </c>
       <c r="N5">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P5" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["秋田県",1],</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="O5">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["秋田",1],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>43898</v>
       </c>
@@ -806,20 +832,24 @@
       <c r="L6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M6" t="e">
-        <f t="shared" si="4"/>
+      <c r="M6" t="str">
+        <f t="shared" si="4"/>
+        <v>山形</v>
+      </c>
+      <c r="N6" t="e">
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="N6">
-        <f t="shared" si="5"/>
+      <c r="O6">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P6" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["山形県",0],</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q6" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["山形",0],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>43898</v>
       </c>
@@ -848,20 +878,24 @@
       <c r="L7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M7">
-        <f t="shared" si="4"/>
-        <v>1</v>
+      <c r="M7" t="str">
+        <f t="shared" si="4"/>
+        <v>福島</v>
       </c>
       <c r="N7">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P7" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["福島県",1],</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="O7">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["福島",1],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>43898</v>
       </c>
@@ -890,20 +924,24 @@
       <c r="L8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="M8" t="e">
-        <f t="shared" si="4"/>
+      <c r="M8" t="str">
+        <f t="shared" si="4"/>
+        <v>茨城</v>
+      </c>
+      <c r="N8" t="e">
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="N8">
-        <f t="shared" si="5"/>
+      <c r="O8">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P8" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["茨城県",0],</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q8" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["茨城",0],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>43898</v>
       </c>
@@ -932,20 +970,24 @@
       <c r="L9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M9">
-        <f t="shared" si="4"/>
+      <c r="M9" t="str">
+        <f t="shared" si="4"/>
+        <v>栃木</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="N9">
-        <f t="shared" si="5"/>
+      <c r="O9">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="P9" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["栃木県",2],</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q9" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["栃木",2],</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>43898</v>
       </c>
@@ -974,20 +1016,24 @@
       <c r="L10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M10">
-        <f t="shared" si="4"/>
-        <v>1</v>
+      <c r="M10" t="str">
+        <f t="shared" si="4"/>
+        <v>群馬</v>
       </c>
       <c r="N10">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P10" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["群馬県",1],</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="O10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["群馬",1],</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>43898</v>
       </c>
@@ -1016,20 +1062,24 @@
       <c r="L11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M11">
-        <f t="shared" si="4"/>
+      <c r="M11" t="str">
+        <f t="shared" si="4"/>
+        <v>埼玉</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="N11">
-        <f t="shared" si="5"/>
+      <c r="O11">
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="P11" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["埼玉県",4],</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q11" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["埼玉",4],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>43898</v>
       </c>
@@ -1058,20 +1108,24 @@
       <c r="L12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M12">
-        <f t="shared" si="4"/>
+      <c r="M12" t="str">
+        <f t="shared" si="4"/>
+        <v>千葉</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="N12">
-        <f t="shared" si="5"/>
+      <c r="O12">
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="P12" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["千葉県",20],</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q12" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["千葉",20],</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>43898</v>
       </c>
@@ -1100,20 +1154,24 @@
       <c r="L13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M13">
-        <f t="shared" si="4"/>
+      <c r="M13" t="str">
+        <f t="shared" si="4"/>
+        <v>東京</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="N13">
-        <f t="shared" si="5"/>
+      <c r="O13">
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="P13" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["東京都",60],</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q13" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["東京",60],</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>43898</v>
       </c>
@@ -1142,20 +1200,24 @@
       <c r="L14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="4"/>
+      <c r="M14" t="str">
+        <f t="shared" si="4"/>
+        <v>神奈川</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
-      <c r="N14">
-        <f t="shared" si="5"/>
+      <c r="O14">
+        <f t="shared" si="6"/>
         <v>34</v>
       </c>
-      <c r="P14" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["神奈川県",34],</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q14" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["神奈川",34],</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>43898</v>
       </c>
@@ -1184,20 +1246,24 @@
       <c r="L15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M15">
-        <f t="shared" si="4"/>
+      <c r="M15" t="str">
+        <f t="shared" si="4"/>
+        <v>新潟</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="N15">
-        <f t="shared" si="5"/>
+      <c r="O15">
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="P15" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["新潟県",6],</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q15" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["新潟",6],</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>43898</v>
       </c>
@@ -1226,20 +1292,24 @@
       <c r="L16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="M16" t="e">
-        <f t="shared" si="4"/>
+      <c r="M16" t="str">
+        <f t="shared" si="4"/>
+        <v>富山</v>
+      </c>
+      <c r="N16" t="e">
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="N16">
-        <f t="shared" si="5"/>
+      <c r="O16">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P16" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["富山県",0],</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q16" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["富山",0],</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>43898</v>
       </c>
@@ -1268,20 +1338,24 @@
       <c r="L17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M17">
-        <f t="shared" si="4"/>
+      <c r="M17" t="str">
+        <f t="shared" si="4"/>
+        <v>石川</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="N17">
-        <f t="shared" si="5"/>
+      <c r="O17">
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="P17" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["石川県",4],</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q17" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["石川",4],</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>43898</v>
       </c>
@@ -1310,20 +1384,24 @@
       <c r="L18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="M18" t="e">
-        <f t="shared" si="4"/>
+      <c r="M18" t="str">
+        <f t="shared" si="4"/>
+        <v>福井</v>
+      </c>
+      <c r="N18" t="e">
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="N18">
-        <f t="shared" si="5"/>
+      <c r="O18">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P18" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["福井県",0],</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q18" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["福井",0],</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>43898</v>
       </c>
@@ -1352,20 +1430,24 @@
       <c r="L19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M19">
-        <f t="shared" si="4"/>
+      <c r="M19" t="str">
+        <f t="shared" si="4"/>
+        <v>山梨</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="N19">
-        <f t="shared" si="5"/>
+      <c r="O19">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="P19" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["山梨県",2],</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q19" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["山梨",2],</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>43898</v>
       </c>
@@ -1394,20 +1476,24 @@
       <c r="L20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M20">
-        <f t="shared" si="4"/>
+      <c r="M20" t="str">
+        <f t="shared" si="4"/>
+        <v>長野</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="N20">
-        <f t="shared" si="5"/>
+      <c r="O20">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="P20" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["長野県",2],</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q20" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["長野",2],</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>43898</v>
       </c>
@@ -1436,20 +1522,24 @@
       <c r="L21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M21">
-        <f t="shared" si="4"/>
+      <c r="M21" t="str">
+        <f t="shared" si="4"/>
+        <v>岐阜</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="N21">
-        <f t="shared" si="5"/>
+      <c r="O21">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="P21" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["岐阜県",2],</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q21" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["岐阜",2],</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>43898</v>
       </c>
@@ -1478,20 +1568,24 @@
       <c r="L22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M22">
-        <f t="shared" si="4"/>
-        <v>1</v>
+      <c r="M22" t="str">
+        <f t="shared" si="4"/>
+        <v>静岡</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P22" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["静岡県",1],</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="O22">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q22" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["静岡",1],</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>43898</v>
       </c>
@@ -1520,20 +1614,24 @@
       <c r="L23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M23">
-        <f t="shared" si="4"/>
+      <c r="M23" t="str">
+        <f t="shared" si="4"/>
+        <v>愛知</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="5"/>
         <v>68</v>
       </c>
-      <c r="N23">
-        <f t="shared" si="5"/>
+      <c r="O23">
+        <f t="shared" si="6"/>
         <v>68</v>
       </c>
-      <c r="P23" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["愛知県",68],</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q23" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["愛知",68],</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>43898</v>
       </c>
@@ -1562,20 +1660,24 @@
       <c r="L24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M24">
-        <f t="shared" si="4"/>
-        <v>1</v>
+      <c r="M24" t="str">
+        <f t="shared" si="4"/>
+        <v>三重</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P24" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["三重県",1],</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="O24">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q24" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["三重",1],</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>43898</v>
       </c>
@@ -1604,20 +1706,24 @@
       <c r="L25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M25">
-        <f t="shared" si="4"/>
-        <v>1</v>
+      <c r="M25" t="str">
+        <f t="shared" si="4"/>
+        <v>滋賀</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P25" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["滋賀県",1],</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="O25">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q25" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["滋賀",1],</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A26" s="1">
         <v>43898</v>
       </c>
@@ -1646,20 +1752,24 @@
       <c r="L26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M26">
-        <f t="shared" si="4"/>
+      <c r="M26" t="str">
+        <f t="shared" si="4"/>
+        <v>京都</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="N26">
-        <f t="shared" si="5"/>
+      <c r="O26">
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="P26" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["京都府",8],</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q26" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["京都",8],</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <v>43898</v>
       </c>
@@ -1688,20 +1798,24 @@
       <c r="L27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M27">
-        <f t="shared" si="4"/>
+      <c r="M27" t="str">
+        <f t="shared" si="4"/>
+        <v>大阪</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
-      <c r="N27">
-        <f t="shared" si="5"/>
+      <c r="O27">
+        <f t="shared" si="6"/>
         <v>33</v>
       </c>
-      <c r="P27" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["大阪府",33],</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q27" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["大阪",33],</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <v>43898</v>
       </c>
@@ -1730,20 +1844,24 @@
       <c r="L28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M28">
-        <f t="shared" si="4"/>
+      <c r="M28" t="str">
+        <f t="shared" si="4"/>
+        <v>兵庫</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="N28">
-        <f t="shared" si="5"/>
+      <c r="O28">
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="P28" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["兵庫県",9],</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q28" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["兵庫",9],</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <v>43898</v>
       </c>
@@ -1772,20 +1890,24 @@
       <c r="L29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M29">
-        <f t="shared" si="4"/>
+      <c r="M29" t="str">
+        <f t="shared" si="4"/>
+        <v>奈良</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="N29">
-        <f t="shared" si="5"/>
+      <c r="O29">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="P29" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["奈良県",2],</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.4">
+      <c r="Q29" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["奈良",2],</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="30" x14ac:dyDescent="0.4">
       <c r="A30" s="1">
         <v>43898</v>
       </c>
@@ -1814,20 +1936,24 @@
       <c r="L30" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M30">
-        <f t="shared" si="4"/>
+      <c r="M30" t="str">
+        <f t="shared" si="4"/>
+        <v>和歌山</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="N30">
-        <f t="shared" si="5"/>
+      <c r="O30">
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="P30" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["和歌山県",12],</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q30" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["和歌山",12],</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <v>43898</v>
       </c>
@@ -1856,20 +1982,24 @@
       <c r="L31" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M31" t="e">
-        <f t="shared" si="4"/>
+      <c r="M31" t="str">
+        <f t="shared" si="4"/>
+        <v>鳥取</v>
+      </c>
+      <c r="N31" t="e">
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="N31">
-        <f t="shared" si="5"/>
+      <c r="O31">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P31" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["鳥取県",0],</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q31" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["鳥取",0],</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
         <v>43898</v>
       </c>
@@ -1898,20 +2028,24 @@
       <c r="L32" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M32" t="e">
-        <f t="shared" si="4"/>
+      <c r="M32" t="str">
+        <f t="shared" si="4"/>
+        <v>島根</v>
+      </c>
+      <c r="N32" t="e">
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="N32">
-        <f t="shared" si="5"/>
+      <c r="O32">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P32" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["島根県",0],</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q32" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["島根",0],</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <v>43898</v>
       </c>
@@ -1940,255 +2074,315 @@
       <c r="L33" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="M33" t="e">
-        <f t="shared" si="4"/>
+      <c r="M33" t="str">
+        <f t="shared" si="4"/>
+        <v>岡山</v>
+      </c>
+      <c r="N33" t="e">
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="N33">
-        <f t="shared" si="5"/>
+      <c r="O33">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P33" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["岡山県",0],</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q33" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["岡山",0],</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L34" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M34">
-        <f t="shared" si="4"/>
-        <v>1</v>
+      <c r="M34" t="str">
+        <f t="shared" si="4"/>
+        <v>広島</v>
       </c>
       <c r="N34">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P34" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["広島県",1],</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="O34">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["広島",1],</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L35" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M35">
-        <f t="shared" si="4"/>
-        <v>1</v>
+      <c r="M35" t="str">
+        <f t="shared" si="4"/>
+        <v>山口</v>
       </c>
       <c r="N35">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P35" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["山口県",1],</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="O35">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q35" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["山口",1],</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M36" t="e">
-        <f t="shared" si="4"/>
+      <c r="M36" t="str">
+        <f t="shared" si="4"/>
+        <v>徳島</v>
+      </c>
+      <c r="N36" t="e">
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="N36">
-        <f t="shared" si="5"/>
+      <c r="O36">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P36" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["徳島県",0],</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q36" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["徳島",0],</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L37" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="M37" t="e">
-        <f t="shared" si="4"/>
+      <c r="M37" t="str">
+        <f t="shared" si="4"/>
+        <v>香川</v>
+      </c>
+      <c r="N37" t="e">
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="N37">
-        <f t="shared" si="5"/>
+      <c r="O37">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P37" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["香川県",0],</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q37" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["香川",0],</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L38" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M38">
-        <f t="shared" si="4"/>
-        <v>1</v>
+      <c r="M38" t="str">
+        <f t="shared" si="4"/>
+        <v>愛媛</v>
       </c>
       <c r="N38">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P38" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["愛媛県",1],</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="O38">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q38" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["愛媛",1],</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L39" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="M39">
-        <f t="shared" si="4"/>
+      <c r="M39" t="str">
+        <f t="shared" si="4"/>
+        <v>高知</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="N39">
-        <f t="shared" si="5"/>
+      <c r="O39">
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="P39" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["高知県",9],</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q39" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["高知",9],</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L40" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="M40">
-        <f t="shared" si="4"/>
+      <c r="M40" t="str">
+        <f t="shared" si="4"/>
+        <v>福岡</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="N40">
-        <f t="shared" si="5"/>
+      <c r="O40">
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="P40" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["福岡県",3],</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q40" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["福岡",3],</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L41" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="M41" t="e">
-        <f t="shared" si="4"/>
+      <c r="M41" t="str">
+        <f t="shared" si="4"/>
+        <v>佐賀</v>
+      </c>
+      <c r="N41" t="e">
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="N41">
-        <f t="shared" si="5"/>
+      <c r="O41">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P41" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["佐賀県",0],</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q41" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["佐賀",0],</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L42" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="M42" t="e">
-        <f t="shared" si="4"/>
+      <c r="M42" t="str">
+        <f t="shared" si="4"/>
+        <v>長崎</v>
+      </c>
+      <c r="N42" t="e">
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="N42">
-        <f t="shared" si="5"/>
+      <c r="O42">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P42" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["長崎県",0],</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q42" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["長崎",0],</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L43" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M43">
-        <f t="shared" si="4"/>
+      <c r="M43" t="str">
+        <f t="shared" si="4"/>
+        <v>熊本</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="N43">
-        <f t="shared" si="5"/>
+      <c r="O43">
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="P43" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["熊本県",5],</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q43" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["熊本",5],</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L44" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="M44">
-        <f t="shared" si="4"/>
-        <v>1</v>
+      <c r="M44" t="str">
+        <f t="shared" si="4"/>
+        <v>大分</v>
       </c>
       <c r="N44">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P44" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["大分県",1],</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="O44">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q44" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["大分",1],</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L45" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M45">
-        <f t="shared" si="4"/>
-        <v>1</v>
+      <c r="M45" t="str">
+        <f t="shared" si="4"/>
+        <v>宮崎</v>
       </c>
       <c r="N45">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P45" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["宮崎県",1],</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" ht="30" x14ac:dyDescent="0.4">
+      <c r="O45">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q45" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["宮崎",1],</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="30" x14ac:dyDescent="0.4">
       <c r="L46" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="M46" t="e">
-        <f t="shared" si="4"/>
+      <c r="M46" t="str">
+        <f t="shared" si="4"/>
+        <v>鹿児島</v>
+      </c>
+      <c r="N46" t="e">
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="N46">
-        <f t="shared" si="5"/>
+      <c r="O46">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P46" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["鹿児島県",0],</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="Q46" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["鹿児島",0],</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L47" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M47">
-        <f t="shared" si="4"/>
+      <c r="M47" t="str">
+        <f t="shared" si="4"/>
+        <v>沖縄</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="N47">
-        <f t="shared" si="5"/>
+      <c r="O47">
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="P47" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">      ["沖縄県",3],</v>
+      <c r="Q47" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">      ["沖縄",3],</v>
       </c>
     </row>
   </sheetData>
@@ -2694,12 +2888,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2912,15 +3103,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44593F81-3CCA-4F6E-9947-5EA7D2ADD190}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{801B1D82-B996-4A37-80BD-D897B90C5E49}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="20ae0c58-a6a6-4144-9137-10cd87cf16fa"/>
+    <ds:schemaRef ds:uri="605e9124-c22f-4077-8c7b-4a5976888914"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2945,18 +3148,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{801B1D82-B996-4A37-80BD-D897B90C5E49}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44593F81-3CCA-4F6E-9947-5EA7D2ADD190}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="20ae0c58-a6a6-4144-9137-10cd87cf16fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="605e9124-c22f-4077-8c7b-4a5976888914"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>